<commit_message>
Correction to one codetype in procedure code list
</commit_message>
<xml_diff>
--- a/mhrn_procedure_codes_new2025.xlsx
+++ b/mhrn_procedure_codes_new2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MH_VDW\gitRepo\MHRN-Central-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C1781E-F3AD-422D-AA78-7ED8672AB153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992ACDB-A6E4-42EF-9D35-8191C6A0FE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="10104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mhpx_codelist_new" sheetId="1" r:id="rId1"/>
@@ -1262,18 +1262,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>90785</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>90791</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>90792</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>90801</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>90802</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>90804</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>90805</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>90806</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>90807</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>90808</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>90809</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>90810</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>90811</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>90812</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>90813</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>90814</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>90815</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>90816</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>90817</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>90818</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>90819</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>90820</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>90821</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>90822</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>90823</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>90826</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>90827</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>90828</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>90832</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>90833</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>90834</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>90836</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>90837</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>90838</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>90839</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>90840</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>90844</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>90845</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>90846</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>90847</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>90849</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>90853</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>90857</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>90862</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>90863</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>90867</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>90868</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>90869</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>90870</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>90875</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>90876</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>90880</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>90882</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>90885</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>90887</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>90889</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>90899</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>97</v>
       </c>
@@ -2856,10 +2856,10 @@
         <v>98</v>
       </c>
       <c r="E73" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>99</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>101</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>103</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>105</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>107</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>109</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>111</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>113</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>115</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>117</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>119</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>121</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>123</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>125</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>127</v>
       </c>

</xml_diff>